<commit_message>
Updated stats with Spark streaming
</commit_message>
<xml_diff>
--- a/stats_raw.xlsx
+++ b/stats_raw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Google Drive\code\DSProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="26">
   <si>
     <t>CPU0</t>
   </si>
@@ -100,13 +100,16 @@
   <si>
     <t>Flink (Batch)</t>
   </si>
+  <si>
+    <t>Spark (Stream)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -150,8 +153,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W41"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="V38" sqref="V38:V41"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45:J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3014,6 +3017,709 @@
         <v>2346.2400000000002</v>
       </c>
     </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A43" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M44" t="s">
+        <v>1</v>
+      </c>
+      <c r="N44" t="s">
+        <v>3</v>
+      </c>
+      <c r="O44" t="s">
+        <v>5</v>
+      </c>
+      <c r="P44" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>9</v>
+      </c>
+      <c r="R44" t="s">
+        <v>11</v>
+      </c>
+      <c r="S44" t="s">
+        <v>13</v>
+      </c>
+      <c r="T44" t="s">
+        <v>15</v>
+      </c>
+      <c r="U44" t="s">
+        <v>17</v>
+      </c>
+      <c r="V44" t="s">
+        <v>19</v>
+      </c>
+      <c r="W44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A45" s="1">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0</v>
+      </c>
+      <c r="K45" s="5">
+        <f>AVERAGE(A45:J45)</f>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="M45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="N45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="O45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="P45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="R45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="S45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="T45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="U45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="V45" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="W45" s="3">
+        <f>AVERAGE(M45:V45)*1024</f>
+        <v>95.129599999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A46" s="1">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0.432</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="K46" s="5">
+        <f>AVERAGE(A46:J46)</f>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="M46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="N46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="O46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="P46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="R46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="S46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="T46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="U46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="V46" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="W46" s="3">
+        <f>AVERAGE(M46:V46)*1024</f>
+        <v>95.129599999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A47" s="1">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="H47" s="1">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1</v>
+      </c>
+      <c r="K47" s="5">
+        <f>AVERAGE(A47:J47)</f>
+        <v>0.99909999999999999</v>
+      </c>
+      <c r="M47" s="1">
+        <v>0.24440000000000001</v>
+      </c>
+      <c r="N47" s="1">
+        <v>0.2424</v>
+      </c>
+      <c r="O47" s="1">
+        <v>0.21920000000000001</v>
+      </c>
+      <c r="P47" s="1">
+        <v>0.2455</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>0.24340000000000001</v>
+      </c>
+      <c r="R47" s="1">
+        <v>0.21920000000000001</v>
+      </c>
+      <c r="S47" s="1">
+        <v>0.2505</v>
+      </c>
+      <c r="T47" s="1">
+        <v>0.24340000000000001</v>
+      </c>
+      <c r="U47" s="1">
+        <v>0.17169999999999999</v>
+      </c>
+      <c r="V47" s="1">
+        <v>0.22320000000000001</v>
+      </c>
+      <c r="W47" s="3">
+        <f>AVERAGE(M47:V47)*1024</f>
+        <v>235.81696000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A48" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.755</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="I48" s="1">
+        <v>1</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="K48" s="5">
+        <f>AVERAGE(A48:J48)</f>
+        <v>0.85660000000000003</v>
+      </c>
+      <c r="M48" s="1">
+        <v>0.38279999999999997</v>
+      </c>
+      <c r="N48" s="1">
+        <v>0.37580000000000002</v>
+      </c>
+      <c r="O48" s="1">
+        <v>0.36770000000000003</v>
+      </c>
+      <c r="P48" s="1">
+        <v>0.37580000000000002</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>0.37680000000000002</v>
+      </c>
+      <c r="R48" s="1">
+        <v>0.36570000000000003</v>
+      </c>
+      <c r="S48" s="1">
+        <v>0.38990000000000002</v>
+      </c>
+      <c r="T48" s="1">
+        <v>0.37880000000000003</v>
+      </c>
+      <c r="U48" s="1">
+        <v>0.33029999999999998</v>
+      </c>
+      <c r="V48" s="1">
+        <v>0.36770000000000003</v>
+      </c>
+      <c r="W48" s="3">
+        <f>AVERAGE(M48:V48)*1024</f>
+        <v>380.03712000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A49" s="1">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="B49" s="1">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C49" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="F49" s="1">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G49" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H49" s="1">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="J49" s="1">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="K49" s="5">
+        <f>AVERAGE(A49:J49)</f>
+        <v>8.6699999999999999E-2</v>
+      </c>
+      <c r="M49" s="1">
+        <v>0.43940000000000001</v>
+      </c>
+      <c r="N49" s="1">
+        <v>0.4788</v>
+      </c>
+      <c r="O49" s="1">
+        <v>0.44950000000000001</v>
+      </c>
+      <c r="P49" s="1">
+        <v>0.45150000000000001</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>0.45450000000000002</v>
+      </c>
+      <c r="R49" s="1">
+        <v>0.44850000000000001</v>
+      </c>
+      <c r="S49" s="1">
+        <v>0.44650000000000001</v>
+      </c>
+      <c r="T49" s="1">
+        <v>0.4657</v>
+      </c>
+      <c r="U49" s="1">
+        <v>0.37880000000000003</v>
+      </c>
+      <c r="V49" s="1">
+        <v>0.44240000000000002</v>
+      </c>
+      <c r="W49" s="3">
+        <f>AVERAGE(M49:V49)*1024</f>
+        <v>456.25344000000007</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A50" s="1">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C50" s="1">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H50" s="1">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="K50" s="5">
+        <f>AVERAGE(A50:J50)</f>
+        <v>5.4000000000000006E-2</v>
+      </c>
+      <c r="M50" s="1">
+        <v>0.4556</v>
+      </c>
+      <c r="N50" s="1">
+        <v>0.4929</v>
+      </c>
+      <c r="O50" s="1">
+        <v>0.45660000000000001</v>
+      </c>
+      <c r="P50" s="1">
+        <v>0.46970000000000001</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>0.4758</v>
+      </c>
+      <c r="R50" s="1">
+        <v>0.46870000000000001</v>
+      </c>
+      <c r="S50" s="1">
+        <v>0.4677</v>
+      </c>
+      <c r="T50" s="1">
+        <v>0.4778</v>
+      </c>
+      <c r="U50" s="1">
+        <v>0.4556</v>
+      </c>
+      <c r="V50" s="1">
+        <v>0.46160000000000001</v>
+      </c>
+      <c r="W50" s="3">
+        <f>AVERAGE(M50:V50)*1024</f>
+        <v>479.43679999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A51" s="1">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="B51" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.753</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="I51" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="K51" s="5">
+        <f>AVERAGE(A51:J51)</f>
+        <v>0.49119999999999997</v>
+      </c>
+      <c r="M51" s="1">
+        <v>0.46970000000000001</v>
+      </c>
+      <c r="N51" s="1">
+        <v>0.5071</v>
+      </c>
+      <c r="O51" s="1">
+        <v>0.47370000000000001</v>
+      </c>
+      <c r="P51" s="1">
+        <v>0.48380000000000001</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>0.4909</v>
+      </c>
+      <c r="R51" s="1">
+        <v>0.48380000000000001</v>
+      </c>
+      <c r="S51" s="1">
+        <v>0.48280000000000001</v>
+      </c>
+      <c r="T51" s="1">
+        <v>0.4919</v>
+      </c>
+      <c r="U51" s="1">
+        <v>0.47170000000000001</v>
+      </c>
+      <c r="V51" s="1">
+        <v>0.4798</v>
+      </c>
+      <c r="W51" s="3">
+        <f>AVERAGE(M51:V51)*1024</f>
+        <v>495.12448000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A52" s="1">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F52" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="J52" s="1">
+        <v>6.3E-2</v>
+      </c>
+      <c r="K52" s="5">
+        <f>AVERAGE(A52:J52)</f>
+        <v>0.32709999999999995</v>
+      </c>
+      <c r="M52" s="1">
+        <v>0.4869</v>
+      </c>
+      <c r="N52" s="1">
+        <v>0.53639999999999999</v>
+      </c>
+      <c r="O52" s="1">
+        <v>0.56059999999999999</v>
+      </c>
+      <c r="P52" s="1">
+        <v>0.55249999999999999</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>0.55659999999999998</v>
+      </c>
+      <c r="R52" s="1">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="S52" s="1">
+        <v>0.55349999999999999</v>
+      </c>
+      <c r="T52" s="1">
+        <v>0.55149999999999999</v>
+      </c>
+      <c r="U52" s="1">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="V52" s="1">
+        <v>0.55149999999999999</v>
+      </c>
+      <c r="W52" s="3">
+        <f>AVERAGE(M52:V52)*1024</f>
+        <v>551.92575999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A53" s="1">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0</v>
+      </c>
+      <c r="K53" s="5">
+        <f>AVERAGE(A53:J53)</f>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="M53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="N53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="O53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="P53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="R53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="S53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="T53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="U53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="V53" s="1">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="W53" s="3">
+        <f>AVERAGE(M53:V53)*1024</f>
+        <v>95.129599999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated stats with Storm
</commit_message>
<xml_diff>
--- a/stats_raw.xlsx
+++ b/stats_raw.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="27">
   <si>
     <t>CPU0</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Spark (Stream)</t>
+  </si>
+  <si>
+    <t>Storm</t>
   </si>
 </sst>
 </file>
@@ -470,16 +473,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:W84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45:J53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="S83" sqref="S83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="10" width="10.6640625" style="4"/>
-    <col min="11" max="12" width="10.6640625" style="2"/>
+    <col min="11" max="11" width="10.6640625" style="5"/>
+    <col min="12" max="12" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.45">
@@ -518,7 +522,7 @@
       <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M2" t="s">
@@ -2131,7 +2135,7 @@
       <c r="J27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M27" t="s">
@@ -2659,7 +2663,6 @@
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="K35" s="5"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="W35" s="3"/>
@@ -2700,7 +2703,7 @@
       <c r="J37" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="K37" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M37" t="s">
@@ -2756,16 +2759,16 @@
       <c r="F38" s="4">
         <v>0</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="4">
         <v>0</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="4">
         <v>0</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="4">
         <v>0</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="4">
         <v>0</v>
       </c>
       <c r="K38" s="5">
@@ -2826,16 +2829,16 @@
       <c r="F39" s="4">
         <v>0.69399999999999995</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="4">
         <v>0.45700000000000002</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="4">
         <v>0.63700000000000001</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="4">
         <v>0.67800000000000005</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="4">
         <v>0.71299999999999997</v>
       </c>
       <c r="K39" s="5">
@@ -2896,16 +2899,16 @@
       <c r="F40" s="4">
         <v>0.23100000000000001</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="4">
         <v>0.441</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="4">
         <v>0.19600000000000001</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="4">
         <v>0.32900000000000001</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40" s="4">
         <v>0.28000000000000003</v>
       </c>
       <c r="K40" s="5">
@@ -2966,16 +2969,16 @@
       <c r="F41" s="4">
         <v>2E-3</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="4">
         <v>2E-3</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="4">
         <v>2E-3</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="4">
         <v>2E-3</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J41" s="4">
         <v>0</v>
       </c>
       <c r="K41" s="5">
@@ -3053,7 +3056,7 @@
       <c r="J44" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="K44" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M44" t="s">
@@ -3091,38 +3094,38 @@
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A45" s="1">
+      <c r="A45" s="4">
         <v>0</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="4">
         <v>0</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="4">
         <v>0</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="4">
         <v>0</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G45" s="4">
         <v>0</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45" s="4">
         <v>0</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I45" s="4">
         <v>0</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45" s="4">
         <v>0</v>
       </c>
       <c r="K45" s="5">
-        <f>AVERAGE(A45:J45)</f>
+        <f t="shared" ref="K45:K53" si="6">AVERAGE(A45:J45)</f>
         <v>6.0000000000000006E-4</v>
       </c>
       <c r="M45" s="1">
@@ -3156,43 +3159,43 @@
         <v>9.2899999999999996E-2</v>
       </c>
       <c r="W45" s="3">
-        <f>AVERAGE(M45:V45)*1024</f>
+        <f t="shared" ref="W45:W53" si="7">AVERAGE(M45:V45)*1024</f>
         <v>95.129599999999996</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A46" s="1">
+      <c r="A46" s="4">
         <v>0.81699999999999995</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="4">
         <v>0.79700000000000004</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="4">
         <v>0.68899999999999995</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="4">
         <v>0.79100000000000004</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="4">
         <v>0.81299999999999994</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="4">
         <v>0.67700000000000005</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="4">
         <v>0.82399999999999995</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="4">
         <v>0.79500000000000004</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46" s="4">
         <v>0.432</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46" s="4">
         <v>0.72499999999999998</v>
       </c>
       <c r="K46" s="5">
-        <f>AVERAGE(A46:J46)</f>
+        <f t="shared" si="6"/>
         <v>0.73599999999999999</v>
       </c>
       <c r="M46" s="1">
@@ -3226,43 +3229,43 @@
         <v>9.2899999999999996E-2</v>
       </c>
       <c r="W46" s="3">
-        <f>AVERAGE(M46:V46)*1024</f>
+        <f t="shared" si="7"/>
         <v>95.129599999999996</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A47" s="1">
-        <v>1</v>
-      </c>
-      <c r="B47" s="1">
+      <c r="A47" s="4">
+        <v>1</v>
+      </c>
+      <c r="B47" s="4">
         <v>0.997</v>
       </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1">
-        <v>1</v>
-      </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1">
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <v>1</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1</v>
+      </c>
+      <c r="F47" s="4">
+        <v>1</v>
+      </c>
+      <c r="G47" s="4">
         <v>0.997</v>
       </c>
-      <c r="H47" s="1">
-        <v>1</v>
-      </c>
-      <c r="I47" s="1">
+      <c r="H47" s="4">
+        <v>1</v>
+      </c>
+      <c r="I47" s="4">
         <v>0.997</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47" s="4">
         <v>1</v>
       </c>
       <c r="K47" s="5">
-        <f>AVERAGE(A47:J47)</f>
+        <f t="shared" si="6"/>
         <v>0.99909999999999999</v>
       </c>
       <c r="M47" s="1">
@@ -3296,43 +3299,43 @@
         <v>0.22320000000000001</v>
       </c>
       <c r="W47" s="3">
-        <f>AVERAGE(M47:V47)*1024</f>
+        <f t="shared" si="7"/>
         <v>235.81696000000002</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A48" s="1">
+      <c r="A48" s="4">
         <v>0.62</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="4">
         <v>0.92300000000000004</v>
       </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1">
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
         <v>0.92</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="4">
         <v>0.755</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="4">
         <v>0.91600000000000004</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G48" s="4">
         <v>0.68</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H48" s="4">
         <v>0.81899999999999995</v>
       </c>
-      <c r="I48" s="1">
-        <v>1</v>
-      </c>
-      <c r="J48" s="1">
+      <c r="I48" s="4">
+        <v>1</v>
+      </c>
+      <c r="J48" s="4">
         <v>0.93300000000000005</v>
       </c>
       <c r="K48" s="5">
-        <f>AVERAGE(A48:J48)</f>
+        <f t="shared" si="6"/>
         <v>0.85660000000000003</v>
       </c>
       <c r="M48" s="1">
@@ -3366,43 +3369,43 @@
         <v>0.36770000000000003</v>
       </c>
       <c r="W48" s="3">
-        <f>AVERAGE(M48:V48)*1024</f>
+        <f t="shared" si="7"/>
         <v>380.03712000000002</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A49" s="1">
+      <c r="A49" s="4">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="4">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="4">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="4">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="4">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="4">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H49" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49" s="4">
         <v>0.23</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J49" s="4">
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="K49" s="5">
-        <f>AVERAGE(A49:J49)</f>
+        <f t="shared" si="6"/>
         <v>8.6699999999999999E-2</v>
       </c>
       <c r="M49" s="1">
@@ -3436,43 +3439,43 @@
         <v>0.44240000000000002</v>
       </c>
       <c r="W49" s="3">
-        <f>AVERAGE(M49:V49)*1024</f>
+        <f t="shared" si="7"/>
         <v>456.25344000000007</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A50" s="1">
+      <c r="A50" s="4">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="4">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="4">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="4">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="4">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50" s="4">
         <v>0.05</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50" s="4">
         <v>0.05</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50" s="4">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50" s="4">
         <v>0.05</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J50" s="4">
         <v>0.06</v>
       </c>
       <c r="K50" s="5">
-        <f>AVERAGE(A50:J50)</f>
+        <f t="shared" si="6"/>
         <v>5.4000000000000006E-2</v>
       </c>
       <c r="M50" s="1">
@@ -3506,43 +3509,43 @@
         <v>0.46160000000000001</v>
       </c>
       <c r="W50" s="3">
-        <f>AVERAGE(M50:V50)*1024</f>
+        <f t="shared" si="7"/>
         <v>479.43679999999995</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A51" s="1">
+      <c r="A51" s="4">
         <v>0.14399999999999999</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="4">
         <v>0.68300000000000005</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="4">
         <v>0.63500000000000001</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="4">
         <v>0.753</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="4">
         <v>0.77900000000000003</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51" s="4">
         <v>0.60099999999999998</v>
       </c>
-      <c r="H51" s="1">
+      <c r="H51" s="4">
         <v>0.52</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I51" s="4">
         <v>4.7E-2</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J51" s="4">
         <v>0.65200000000000002</v>
       </c>
       <c r="K51" s="5">
-        <f>AVERAGE(A51:J51)</f>
+        <f t="shared" si="6"/>
         <v>0.49119999999999997</v>
       </c>
       <c r="M51" s="1">
@@ -3576,43 +3579,43 @@
         <v>0.4798</v>
       </c>
       <c r="W51" s="3">
-        <f>AVERAGE(M51:V51)*1024</f>
+        <f t="shared" si="7"/>
         <v>495.12448000000006</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A52" s="1">
+      <c r="A52" s="4">
         <v>0.78400000000000003</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="4">
         <v>0.68100000000000005</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="4">
         <v>0.33700000000000002</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="4">
         <v>0.13300000000000001</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="4">
         <v>0.01</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G52" s="4">
         <v>0.14299999999999999</v>
       </c>
-      <c r="H52" s="1">
+      <c r="H52" s="4">
         <v>0.3</v>
       </c>
-      <c r="I52" s="1">
+      <c r="I52" s="4">
         <v>0.81699999999999995</v>
       </c>
-      <c r="J52" s="1">
+      <c r="J52" s="4">
         <v>6.3E-2</v>
       </c>
       <c r="K52" s="5">
-        <f>AVERAGE(A52:J52)</f>
+        <f t="shared" si="6"/>
         <v>0.32709999999999995</v>
       </c>
       <c r="M52" s="1">
@@ -3646,43 +3649,43 @@
         <v>0.55149999999999999</v>
       </c>
       <c r="W52" s="3">
-        <f>AVERAGE(M52:V52)*1024</f>
+        <f t="shared" si="7"/>
         <v>551.92575999999997</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A53" s="1">
+      <c r="A53" s="4">
         <v>0</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="4">
         <v>0</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="4">
         <v>0</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="4">
         <v>0</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F53" s="4">
         <v>0</v>
       </c>
-      <c r="G53" s="1">
+      <c r="G53" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H53" s="4">
         <v>0</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I53" s="4">
         <v>0</v>
       </c>
-      <c r="J53" s="1">
+      <c r="J53" s="4">
         <v>0</v>
       </c>
       <c r="K53" s="5">
-        <f>AVERAGE(A53:J53)</f>
+        <f t="shared" si="6"/>
         <v>6.0000000000000006E-4</v>
       </c>
       <c r="M53" s="1">
@@ -3716,9 +3719,1976 @@
         <v>9.2899999999999996E-2</v>
       </c>
       <c r="W53" s="3">
-        <f>AVERAGE(M53:V53)*1024</f>
+        <f t="shared" si="7"/>
         <v>95.129599999999996</v>
       </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A55" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56" t="s">
+        <v>1</v>
+      </c>
+      <c r="N56" t="s">
+        <v>3</v>
+      </c>
+      <c r="O56" t="s">
+        <v>5</v>
+      </c>
+      <c r="P56" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>9</v>
+      </c>
+      <c r="R56" t="s">
+        <v>11</v>
+      </c>
+      <c r="S56" t="s">
+        <v>13</v>
+      </c>
+      <c r="T56" t="s">
+        <v>15</v>
+      </c>
+      <c r="U56" t="s">
+        <v>17</v>
+      </c>
+      <c r="V56" t="s">
+        <v>19</v>
+      </c>
+      <c r="W56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A57" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="B57" s="4">
+        <v>0</v>
+      </c>
+      <c r="C57" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K57" s="5">
+        <f t="shared" ref="K57:K84" si="8">AVERAGE(A57:J57)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="M57" s="1">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="N57" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="O57" s="1">
+        <v>1.83E-2</v>
+      </c>
+      <c r="P57" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="R57" s="1">
+        <v>0.1323</v>
+      </c>
+      <c r="S57" s="1">
+        <v>0.17419999999999999</v>
+      </c>
+      <c r="T57" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="U57" s="1">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="V57" s="1">
+        <v>0.1293</v>
+      </c>
+      <c r="W57" s="3">
+        <f>AVERAGE(M57:V57)*3000</f>
+        <v>213.18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A58" s="4">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="B58" s="4">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0.753</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K58" s="5">
+        <f t="shared" si="8"/>
+        <v>0.69689999999999996</v>
+      </c>
+      <c r="M58" s="1">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="N58" s="1">
+        <v>1.83E-2</v>
+      </c>
+      <c r="O58" s="1">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="P58" s="1">
+        <v>1.83E-2</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="R58" s="1">
+        <v>0.1323</v>
+      </c>
+      <c r="S58" s="1">
+        <v>0.17449999999999999</v>
+      </c>
+      <c r="T58" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="U58" s="1">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="V58" s="1">
+        <v>0.1293</v>
+      </c>
+      <c r="W58" s="3">
+        <f t="shared" ref="W58:W84" si="9">AVERAGE(M58:V58)*3000</f>
+        <v>213.54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A59" s="4">
+        <v>1</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1</v>
+      </c>
+      <c r="C59" s="4">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1">
+        <v>1</v>
+      </c>
+      <c r="J59" s="1">
+        <v>1</v>
+      </c>
+      <c r="K59" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M59" s="1">
+        <v>6.9099999999999995E-2</v>
+      </c>
+      <c r="N59" s="1">
+        <v>7.2099999999999997E-2</v>
+      </c>
+      <c r="O59" s="1">
+        <v>7.0099999999999996E-2</v>
+      </c>
+      <c r="P59" s="1">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>0.14660000000000001</v>
+      </c>
+      <c r="R59" s="1">
+        <v>0.1739</v>
+      </c>
+      <c r="S59" s="1">
+        <v>0.20880000000000001</v>
+      </c>
+      <c r="T59" s="1">
+        <v>4.82E-2</v>
+      </c>
+      <c r="U59" s="1">
+        <v>0.1439</v>
+      </c>
+      <c r="V59" s="1">
+        <v>0.18149999999999999</v>
+      </c>
+      <c r="W59" s="3">
+        <f t="shared" si="9"/>
+        <v>355.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A60" s="4">
+        <v>1</v>
+      </c>
+      <c r="B60" s="4">
+        <v>1</v>
+      </c>
+      <c r="C60" s="4">
+        <v>1</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+      <c r="I60" s="1">
+        <v>1</v>
+      </c>
+      <c r="J60" s="1">
+        <v>1</v>
+      </c>
+      <c r="K60" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M60" s="1">
+        <v>9.3799999999999994E-2</v>
+      </c>
+      <c r="N60" s="1">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="O60" s="1">
+        <v>9.4399999999999998E-2</v>
+      </c>
+      <c r="P60" s="1">
+        <v>9.3100000000000002E-2</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>0.1686</v>
+      </c>
+      <c r="R60" s="1">
+        <v>0.20680000000000001</v>
+      </c>
+      <c r="S60" s="1">
+        <v>0.2477</v>
+      </c>
+      <c r="T60" s="1">
+        <v>9.0399999999999994E-2</v>
+      </c>
+      <c r="U60" s="1">
+        <v>0.16619999999999999</v>
+      </c>
+      <c r="V60" s="1">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="W60" s="3">
+        <f t="shared" si="9"/>
+        <v>437.46000000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A61" s="4">
+        <v>1</v>
+      </c>
+      <c r="B61" s="4">
+        <v>1</v>
+      </c>
+      <c r="C61" s="4">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61" s="1">
+        <v>1</v>
+      </c>
+      <c r="J61" s="1">
+        <v>1</v>
+      </c>
+      <c r="K61" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M61" s="1">
+        <v>0.1041</v>
+      </c>
+      <c r="N61" s="1">
+        <v>0.10440000000000001</v>
+      </c>
+      <c r="O61" s="1">
+        <v>0.1037</v>
+      </c>
+      <c r="P61" s="1">
+        <v>0.10539999999999999</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>0.1802</v>
+      </c>
+      <c r="R61" s="1">
+        <v>0.21510000000000001</v>
+      </c>
+      <c r="S61" s="1">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="T61" s="1">
+        <v>0.1004</v>
+      </c>
+      <c r="U61" s="1">
+        <v>0.1769</v>
+      </c>
+      <c r="V61" s="1">
+        <v>0.21510000000000001</v>
+      </c>
+      <c r="W61" s="3">
+        <f t="shared" si="9"/>
+        <v>468.69000000000011</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A62" s="4">
+        <v>1</v>
+      </c>
+      <c r="B62" s="4">
+        <v>1</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
+      <c r="J62" s="1">
+        <v>1</v>
+      </c>
+      <c r="K62" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M62" s="1">
+        <v>0.111</v>
+      </c>
+      <c r="N62" s="1">
+        <v>0.1114</v>
+      </c>
+      <c r="O62" s="1">
+        <v>0.1104</v>
+      </c>
+      <c r="P62" s="1">
+        <v>0.112</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>0.1865</v>
+      </c>
+      <c r="R62" s="1">
+        <v>0.22370000000000001</v>
+      </c>
+      <c r="S62" s="1">
+        <v>0.26529999999999998</v>
+      </c>
+      <c r="T62" s="1">
+        <v>0.1094</v>
+      </c>
+      <c r="U62" s="1">
+        <v>0.18479999999999999</v>
+      </c>
+      <c r="V62" s="1">
+        <v>0.22309999999999999</v>
+      </c>
+      <c r="W62" s="3">
+        <f t="shared" si="9"/>
+        <v>491.28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A63" s="4">
+        <v>1</v>
+      </c>
+      <c r="B63" s="4">
+        <v>1</v>
+      </c>
+      <c r="C63" s="4">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
+      <c r="J63" s="1">
+        <v>1</v>
+      </c>
+      <c r="K63" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M63" s="1">
+        <v>6.9099999999999995E-2</v>
+      </c>
+      <c r="N63" s="1">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="O63" s="1">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="P63" s="1">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="R63" s="1">
+        <v>0.1686</v>
+      </c>
+      <c r="S63" s="1">
+        <v>0.2094</v>
+      </c>
+      <c r="T63" s="1">
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="U63" s="1">
+        <v>0.15260000000000001</v>
+      </c>
+      <c r="V63" s="1">
+        <v>0.1915</v>
+      </c>
+      <c r="W63" s="3">
+        <f t="shared" si="9"/>
+        <v>364.65000000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A64" s="4">
+        <v>1</v>
+      </c>
+      <c r="B64" s="4">
+        <v>1</v>
+      </c>
+      <c r="C64" s="4">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1</v>
+      </c>
+      <c r="I64" s="1">
+        <v>1</v>
+      </c>
+      <c r="J64" s="1">
+        <v>1</v>
+      </c>
+      <c r="K64" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M64" s="1">
+        <v>9.5399999999999999E-2</v>
+      </c>
+      <c r="N64" s="1">
+        <v>9.7100000000000006E-2</v>
+      </c>
+      <c r="O64" s="1">
+        <v>9.5100000000000004E-2</v>
+      </c>
+      <c r="P64" s="1">
+        <v>9.5399999999999999E-2</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>0.1709</v>
+      </c>
+      <c r="R64" s="1">
+        <v>0.20880000000000001</v>
+      </c>
+      <c r="S64" s="1">
+        <v>0.25030000000000002</v>
+      </c>
+      <c r="T64" s="1">
+        <v>9.3799999999999994E-2</v>
+      </c>
+      <c r="U64" s="1">
+        <v>0.1719</v>
+      </c>
+      <c r="V64" s="1">
+        <v>0.2104</v>
+      </c>
+      <c r="W64" s="3">
+        <f t="shared" si="9"/>
+        <v>446.73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A65" s="4">
+        <v>1</v>
+      </c>
+      <c r="B65" s="4">
+        <v>1</v>
+      </c>
+      <c r="C65" s="4">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1">
+        <v>1</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1">
+        <v>1</v>
+      </c>
+      <c r="K65" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M65" s="1">
+        <v>0.1057</v>
+      </c>
+      <c r="N65" s="1">
+        <v>0.107</v>
+      </c>
+      <c r="O65" s="1">
+        <v>0.10639999999999999</v>
+      </c>
+      <c r="P65" s="1">
+        <v>0.1074</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>0.1832</v>
+      </c>
+      <c r="R65" s="1">
+        <v>0.22040000000000001</v>
+      </c>
+      <c r="S65" s="1">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="T65" s="1">
+        <v>0.1061</v>
+      </c>
+      <c r="U65" s="1">
+        <v>0.18149999999999999</v>
+      </c>
+      <c r="V65" s="1">
+        <v>0.21970000000000001</v>
+      </c>
+      <c r="W65" s="3">
+        <f t="shared" si="9"/>
+        <v>479.52000000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A66" s="4">
+        <v>1</v>
+      </c>
+      <c r="B66" s="4">
+        <v>1</v>
+      </c>
+      <c r="C66" s="4">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1">
+        <v>1</v>
+      </c>
+      <c r="H66" s="1">
+        <v>1</v>
+      </c>
+      <c r="I66" s="1">
+        <v>1</v>
+      </c>
+      <c r="J66" s="1">
+        <v>1</v>
+      </c>
+      <c r="K66" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M66" s="1">
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="N66" s="1">
+        <v>6.5799999999999997E-2</v>
+      </c>
+      <c r="O66" s="1">
+        <v>0.1134</v>
+      </c>
+      <c r="P66" s="1">
+        <v>0.1137</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>0.1898</v>
+      </c>
+      <c r="R66" s="1">
+        <v>0.22470000000000001</v>
+      </c>
+      <c r="S66" s="1">
+        <v>0.2676</v>
+      </c>
+      <c r="T66" s="1">
+        <v>0.1137</v>
+      </c>
+      <c r="U66" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="V66" s="1">
+        <v>0.2261</v>
+      </c>
+      <c r="W66" s="3">
+        <f t="shared" si="9"/>
+        <v>466.04999999999995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A67" s="4">
+        <v>1</v>
+      </c>
+      <c r="B67" s="4">
+        <v>1</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1</v>
+      </c>
+      <c r="H67" s="1">
+        <v>1</v>
+      </c>
+      <c r="I67" s="1">
+        <v>1</v>
+      </c>
+      <c r="J67" s="1">
+        <v>1</v>
+      </c>
+      <c r="K67" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M67" s="1">
+        <v>8.0500000000000002E-2</v>
+      </c>
+      <c r="N67" s="1">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="O67" s="1">
+        <v>8.3799999999999999E-2</v>
+      </c>
+      <c r="P67" s="1">
+        <v>9.2100000000000001E-2</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>0.16059999999999999</v>
+      </c>
+      <c r="R67" s="1">
+        <v>0.19409999999999999</v>
+      </c>
+      <c r="S67" s="1">
+        <v>0.2344</v>
+      </c>
+      <c r="T67" s="1">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="U67" s="1">
+        <v>0.16789999999999999</v>
+      </c>
+      <c r="V67" s="1">
+        <v>0.1971</v>
+      </c>
+      <c r="W67" s="3">
+        <f t="shared" si="9"/>
+        <v>415.88999999999993</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A68" s="4">
+        <v>1</v>
+      </c>
+      <c r="B68" s="4">
+        <v>1</v>
+      </c>
+      <c r="C68" s="4">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1">
+        <v>1</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+      <c r="H68" s="1">
+        <v>1</v>
+      </c>
+      <c r="I68" s="1">
+        <v>1</v>
+      </c>
+      <c r="J68" s="1">
+        <v>1</v>
+      </c>
+      <c r="K68" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M68" s="1">
+        <v>9.9099999999999994E-2</v>
+      </c>
+      <c r="N68" s="1">
+        <v>0.1051</v>
+      </c>
+      <c r="O68" s="1">
+        <v>0.1004</v>
+      </c>
+      <c r="P68" s="1">
+        <v>0.1024</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="R68" s="1">
+        <v>0.21240000000000001</v>
+      </c>
+      <c r="S68" s="1">
+        <v>0.252</v>
+      </c>
+      <c r="T68" s="1">
+        <v>9.9400000000000002E-2</v>
+      </c>
+      <c r="U68" s="1">
+        <v>0.1789</v>
+      </c>
+      <c r="V68" s="1">
+        <v>0.21210000000000001</v>
+      </c>
+      <c r="W68" s="3">
+        <f t="shared" si="9"/>
+        <v>461.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A69" s="4">
+        <v>1</v>
+      </c>
+      <c r="B69" s="4">
+        <v>1</v>
+      </c>
+      <c r="C69" s="4">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>1</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+      <c r="I69" s="1">
+        <v>1</v>
+      </c>
+      <c r="J69" s="1">
+        <v>1</v>
+      </c>
+      <c r="K69" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M69" s="1">
+        <v>0.10970000000000001</v>
+      </c>
+      <c r="N69" s="1">
+        <v>0.112</v>
+      </c>
+      <c r="O69" s="1">
+        <v>0.10970000000000001</v>
+      </c>
+      <c r="P69" s="1">
+        <v>0.1104</v>
+      </c>
+      <c r="Q69" s="1">
+        <v>0.1852</v>
+      </c>
+      <c r="R69" s="1">
+        <v>0.22239999999999999</v>
+      </c>
+      <c r="S69" s="1">
+        <v>0.26329999999999998</v>
+      </c>
+      <c r="T69" s="1">
+        <v>0.1084</v>
+      </c>
+      <c r="U69" s="1">
+        <v>0.1862</v>
+      </c>
+      <c r="V69" s="1">
+        <v>0.22209999999999999</v>
+      </c>
+      <c r="W69" s="3">
+        <f t="shared" si="9"/>
+        <v>488.81999999999994</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A70" s="4">
+        <v>1</v>
+      </c>
+      <c r="B70" s="4">
+        <v>1</v>
+      </c>
+      <c r="C70" s="4">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1">
+        <v>1</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1">
+        <v>1</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1</v>
+      </c>
+      <c r="H70" s="1">
+        <v>1</v>
+      </c>
+      <c r="I70" s="1">
+        <v>1</v>
+      </c>
+      <c r="J70" s="1">
+        <v>1</v>
+      </c>
+      <c r="K70" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M70" s="1">
+        <v>4.8899999999999999E-2</v>
+      </c>
+      <c r="N70" s="1">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="O70" s="1">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="P70" s="1">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="R70" s="1">
+        <v>0.15989999999999999</v>
+      </c>
+      <c r="S70" s="1">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="T70" s="1">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="U70" s="1">
+        <v>0.15090000000000001</v>
+      </c>
+      <c r="V70" s="1">
+        <v>0.1729</v>
+      </c>
+      <c r="W70" s="3">
+        <f t="shared" si="9"/>
+        <v>372.71999999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A71" s="4">
+        <v>1</v>
+      </c>
+      <c r="B71" s="4">
+        <v>1</v>
+      </c>
+      <c r="C71" s="4">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1</v>
+      </c>
+      <c r="I71" s="1">
+        <v>1</v>
+      </c>
+      <c r="J71" s="1">
+        <v>1</v>
+      </c>
+      <c r="K71" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M71" s="1">
+        <v>8.7099999999999997E-2</v>
+      </c>
+      <c r="N71" s="1">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="O71" s="1">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="P71" s="1">
+        <v>9.01E-2</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>0.16220000000000001</v>
+      </c>
+      <c r="R71" s="1">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="S71" s="1">
+        <v>0.2364</v>
+      </c>
+      <c r="T71" s="1">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="U71" s="1">
+        <v>0.16819999999999999</v>
+      </c>
+      <c r="V71" s="1">
+        <v>0.2011</v>
+      </c>
+      <c r="W71" s="3">
+        <f t="shared" si="9"/>
+        <v>425.24999999999994</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A72" s="4">
+        <v>1</v>
+      </c>
+      <c r="B72" s="4">
+        <v>1</v>
+      </c>
+      <c r="C72" s="4">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1</v>
+      </c>
+      <c r="H72" s="1">
+        <v>1</v>
+      </c>
+      <c r="I72" s="1">
+        <v>1</v>
+      </c>
+      <c r="J72" s="1">
+        <v>1</v>
+      </c>
+      <c r="K72" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M72" s="1">
+        <v>9.8400000000000001E-2</v>
+      </c>
+      <c r="N72" s="1">
+        <v>0.1031</v>
+      </c>
+      <c r="O72" s="1">
+        <v>0.1011</v>
+      </c>
+      <c r="P72" s="1">
+        <v>9.9099999999999994E-2</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>0.1729</v>
+      </c>
+      <c r="R72" s="1">
+        <v>0.21340000000000001</v>
+      </c>
+      <c r="S72" s="1">
+        <v>0.25130000000000002</v>
+      </c>
+      <c r="T72" s="1">
+        <v>9.7100000000000006E-2</v>
+      </c>
+      <c r="U72" s="1">
+        <v>0.17749999999999999</v>
+      </c>
+      <c r="V72" s="1">
+        <v>0.21240000000000001</v>
+      </c>
+      <c r="W72" s="3">
+        <f t="shared" si="9"/>
+        <v>457.89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A73" s="4">
+        <v>1</v>
+      </c>
+      <c r="B73" s="4">
+        <v>1</v>
+      </c>
+      <c r="C73" s="4">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1</v>
+      </c>
+      <c r="H73" s="1">
+        <v>1</v>
+      </c>
+      <c r="I73" s="1">
+        <v>1</v>
+      </c>
+      <c r="J73" s="1">
+        <v>1</v>
+      </c>
+      <c r="K73" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M73" s="1">
+        <v>0.1087</v>
+      </c>
+      <c r="N73" s="1">
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="O73" s="1">
+        <v>0.108</v>
+      </c>
+      <c r="P73" s="1">
+        <v>0.1077</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="R73" s="1">
+        <v>0.22209999999999999</v>
+      </c>
+      <c r="S73" s="1">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="T73" s="1">
+        <v>0.1061</v>
+      </c>
+      <c r="U73" s="1">
+        <v>0.1845</v>
+      </c>
+      <c r="V73" s="1">
+        <v>0.22070000000000001</v>
+      </c>
+      <c r="W73" s="3">
+        <f t="shared" si="9"/>
+        <v>483.39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A74" s="4">
+        <v>1</v>
+      </c>
+      <c r="B74" s="4">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="C74" s="4">
+        <v>1</v>
+      </c>
+      <c r="D74" s="1">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1">
+        <v>1</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1</v>
+      </c>
+      <c r="H74" s="1">
+        <v>1</v>
+      </c>
+      <c r="I74" s="1">
+        <v>1</v>
+      </c>
+      <c r="J74" s="1">
+        <v>1</v>
+      </c>
+      <c r="K74" s="5">
+        <f t="shared" si="8"/>
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="M74" s="1">
+        <v>0.12230000000000001</v>
+      </c>
+      <c r="N74" s="1">
+        <v>0.13070000000000001</v>
+      </c>
+      <c r="O74" s="1">
+        <v>0.12330000000000001</v>
+      </c>
+      <c r="P74" s="1">
+        <v>0.123</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>0.1948</v>
+      </c>
+      <c r="R74" s="1">
+        <v>0.22939999999999999</v>
+      </c>
+      <c r="S74" s="1">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="T74" s="1">
+        <v>0.1193</v>
+      </c>
+      <c r="U74" s="1">
+        <v>0.2021</v>
+      </c>
+      <c r="V74" s="1">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="W74" s="3">
+        <f t="shared" si="9"/>
+        <v>524.66999999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A75" s="4">
+        <v>0.66</v>
+      </c>
+      <c r="B75" s="4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C75" s="4">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1">
+        <v>1</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0.107</v>
+      </c>
+      <c r="J75" s="1">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="K75" s="5">
+        <f t="shared" si="8"/>
+        <v>0.53559999999999997</v>
+      </c>
+      <c r="M75" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N75" s="1">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="O75" s="1">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="P75" s="1">
+        <v>0.14360000000000001</v>
+      </c>
+      <c r="Q75" s="1">
+        <v>0.21210000000000001</v>
+      </c>
+      <c r="R75" s="1">
+        <v>0.2447</v>
+      </c>
+      <c r="S75" s="1">
+        <v>0.28620000000000001</v>
+      </c>
+      <c r="T75" s="1">
+        <v>0.1366</v>
+      </c>
+      <c r="U75" s="1">
+        <v>0.22339999999999999</v>
+      </c>
+      <c r="V75" s="1">
+        <v>0.255</v>
+      </c>
+      <c r="W75" s="3">
+        <f t="shared" si="9"/>
+        <v>580.04999999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A76" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="B76" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C76" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="F76" s="1">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0.187</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I76" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J76" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K76" s="5">
+        <f t="shared" si="8"/>
+        <v>4.87E-2</v>
+      </c>
+      <c r="M76" s="1">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="N76" s="1">
+        <v>0.1406</v>
+      </c>
+      <c r="O76" s="1">
+        <v>0.1469</v>
+      </c>
+      <c r="P76" s="1">
+        <v>0.14760000000000001</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="R76" s="1">
+        <v>0.2281</v>
+      </c>
+      <c r="S76" s="1">
+        <v>0.30719999999999997</v>
+      </c>
+      <c r="T76" s="1">
+        <v>0.15060000000000001</v>
+      </c>
+      <c r="U76" s="1">
+        <v>0.1832</v>
+      </c>
+      <c r="V76" s="1">
+        <v>0.22070000000000001</v>
+      </c>
+      <c r="W76" s="3">
+        <f t="shared" si="9"/>
+        <v>559.19999999999993</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A77" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="B77" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="C77" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G77" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H77" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I77" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J77" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K77" s="5">
+        <f t="shared" si="8"/>
+        <v>8.9600000000000013E-2</v>
+      </c>
+      <c r="M77" s="1">
+        <v>0.15060000000000001</v>
+      </c>
+      <c r="N77" s="1">
+        <v>0.1406</v>
+      </c>
+      <c r="O77" s="1">
+        <v>0.1386</v>
+      </c>
+      <c r="P77" s="1">
+        <v>0.14760000000000001</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>0.1855</v>
+      </c>
+      <c r="R77" s="1">
+        <v>0.22639999999999999</v>
+      </c>
+      <c r="S77" s="1">
+        <v>0.26329999999999998</v>
+      </c>
+      <c r="T77" s="1">
+        <v>0.14560000000000001</v>
+      </c>
+      <c r="U77" s="1">
+        <v>0.1832</v>
+      </c>
+      <c r="V77" s="1">
+        <v>0.21909999999999999</v>
+      </c>
+      <c r="W77" s="3">
+        <f t="shared" si="9"/>
+        <v>540.15000000000009</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A78" s="4">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="B78" s="4">
+        <v>1</v>
+      </c>
+      <c r="C78" s="4">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="J78" s="1">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="K78" s="5">
+        <f t="shared" si="8"/>
+        <v>0.61219999999999986</v>
+      </c>
+      <c r="M78" s="1">
+        <v>0.15060000000000001</v>
+      </c>
+      <c r="N78" s="1">
+        <v>0.14829999999999999</v>
+      </c>
+      <c r="O78" s="1">
+        <v>0.1386</v>
+      </c>
+      <c r="P78" s="1">
+        <v>0.14760000000000001</v>
+      </c>
+      <c r="Q78" s="1">
+        <v>0.1855</v>
+      </c>
+      <c r="R78" s="1">
+        <v>0.22639999999999999</v>
+      </c>
+      <c r="S78" s="1">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="T78" s="1">
+        <v>0.1459</v>
+      </c>
+      <c r="U78" s="1">
+        <v>0.1835</v>
+      </c>
+      <c r="V78" s="1">
+        <v>0.21909999999999999</v>
+      </c>
+      <c r="W78" s="3">
+        <f t="shared" si="9"/>
+        <v>542.54999999999995</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A79" s="4">
+        <v>0.997</v>
+      </c>
+      <c r="B79" s="4">
+        <v>1</v>
+      </c>
+      <c r="C79" s="4">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="J79" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="K79" s="5">
+        <f t="shared" si="8"/>
+        <v>0.98989999999999989</v>
+      </c>
+      <c r="M79" s="1">
+        <v>0.15290000000000001</v>
+      </c>
+      <c r="N79" s="1">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="O79" s="1">
+        <v>0.14660000000000001</v>
+      </c>
+      <c r="P79" s="1">
+        <v>0.1406</v>
+      </c>
+      <c r="Q79" s="1">
+        <v>0.1915</v>
+      </c>
+      <c r="R79" s="1">
+        <v>0.2324</v>
+      </c>
+      <c r="S79" s="1">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="T79" s="1">
+        <v>0.15129999999999999</v>
+      </c>
+      <c r="U79" s="1">
+        <v>0.1915</v>
+      </c>
+      <c r="V79" s="1">
+        <v>0.22639999999999999</v>
+      </c>
+      <c r="W79" s="3">
+        <f t="shared" si="9"/>
+        <v>553.05000000000007</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A80" s="4">
+        <v>1</v>
+      </c>
+      <c r="B80" s="4">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="C80" s="4">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="J80" s="1">
+        <v>1</v>
+      </c>
+      <c r="K80" s="5">
+        <f t="shared" si="8"/>
+        <v>0.95489999999999997</v>
+      </c>
+      <c r="M80" s="1">
+        <v>0.1416</v>
+      </c>
+      <c r="N80" s="1">
+        <v>0.1449</v>
+      </c>
+      <c r="O80" s="1">
+        <v>0.14560000000000001</v>
+      </c>
+      <c r="P80" s="1">
+        <v>0.15790000000000001</v>
+      </c>
+      <c r="Q80" s="1">
+        <v>0.18920000000000001</v>
+      </c>
+      <c r="R80" s="1">
+        <v>0.2324</v>
+      </c>
+      <c r="S80" s="1">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="T80" s="1">
+        <v>0.14990000000000001</v>
+      </c>
+      <c r="U80" s="1">
+        <v>0.1925</v>
+      </c>
+      <c r="V80" s="1">
+        <v>0.2261</v>
+      </c>
+      <c r="W80" s="3">
+        <f t="shared" si="9"/>
+        <v>555.11999999999989</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A81" s="4">
+        <v>1</v>
+      </c>
+      <c r="B81" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="I81" s="1">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="J81" s="1">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="K81" s="5">
+        <f t="shared" si="8"/>
+        <v>0.70719999999999994</v>
+      </c>
+      <c r="M81" s="1">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="N81" s="1">
+        <v>0.124</v>
+      </c>
+      <c r="O81" s="1">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="P81" s="1">
+        <v>0.15759999999999999</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="R81" s="1">
+        <v>0.22939999999999999</v>
+      </c>
+      <c r="S81" s="1">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="T81" s="1">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="U81" s="1">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="V81" s="1">
+        <v>0.22339999999999999</v>
+      </c>
+      <c r="W81" s="3">
+        <f t="shared" si="9"/>
+        <v>548.16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A82" s="4">
+        <v>0.151</v>
+      </c>
+      <c r="B82" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="C82" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G82" s="1">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="H82" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I82" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J82" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K82" s="5">
+        <f t="shared" si="8"/>
+        <v>8.77E-2</v>
+      </c>
+      <c r="M82" s="1">
+        <v>0.15690000000000001</v>
+      </c>
+      <c r="N82" s="1">
+        <v>9.01E-2</v>
+      </c>
+      <c r="O82" s="1">
+        <v>0.1217</v>
+      </c>
+      <c r="P82" s="1">
+        <v>0.15490000000000001</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>0.1686</v>
+      </c>
+      <c r="R82" s="1">
+        <v>0.21110000000000001</v>
+      </c>
+      <c r="S82" s="1">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="T82" s="1">
+        <v>0.129</v>
+      </c>
+      <c r="U82" s="1">
+        <v>0.16619999999999999</v>
+      </c>
+      <c r="V82" s="1">
+        <v>0.2021</v>
+      </c>
+      <c r="W82" s="3">
+        <f t="shared" si="9"/>
+        <v>500.57999999999993</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A83" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="C83" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E83" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="G83" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="I83" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J83" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K83" s="5">
+        <f t="shared" si="8"/>
+        <v>2.3666666666666669E-2</v>
+      </c>
+      <c r="M83" s="1">
+        <v>0.1333</v>
+      </c>
+      <c r="O83" s="1">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="P83" s="1">
+        <v>9.3799999999999994E-2</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>0.16889999999999999</v>
+      </c>
+      <c r="R83" s="1">
+        <v>0.17349999999999999</v>
+      </c>
+      <c r="S83" s="1">
+        <v>0.2094</v>
+      </c>
+      <c r="T83" s="1">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="U83" s="1">
+        <v>0.1283</v>
+      </c>
+      <c r="V83" s="1">
+        <v>0.16420000000000001</v>
+      </c>
+      <c r="W83" s="3">
+        <f t="shared" si="9"/>
+        <v>417.66666666666674</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="E84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="S84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="W84" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated stats with Flink streaming
</commit_message>
<xml_diff>
--- a/stats_raw.xlsx
+++ b/stats_raw.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="28">
   <si>
     <t>CPU0</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Storm</t>
+  </si>
+  <si>
+    <t>Flink (Stream)</t>
   </si>
 </sst>
 </file>
@@ -473,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W84"/>
+  <dimension ref="A1:W90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="S83" sqref="S83"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="U90" sqref="U90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5690,6 +5693,359 @@
       <c r="V84" s="1"/>
       <c r="W84" s="3"/>
     </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A85" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A86" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K86" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M86" t="s">
+        <v>1</v>
+      </c>
+      <c r="N86" t="s">
+        <v>3</v>
+      </c>
+      <c r="O86" t="s">
+        <v>5</v>
+      </c>
+      <c r="P86" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>9</v>
+      </c>
+      <c r="R86" t="s">
+        <v>11</v>
+      </c>
+      <c r="S86" t="s">
+        <v>13</v>
+      </c>
+      <c r="T86" t="s">
+        <v>15</v>
+      </c>
+      <c r="U86" t="s">
+        <v>17</v>
+      </c>
+      <c r="V86" t="s">
+        <v>19</v>
+      </c>
+      <c r="W86" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A87" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B87" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="C87" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="D87" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="E87" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="F87" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="G87" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H87" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="I87" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="J87" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="K87" s="5">
+        <f t="shared" ref="K87:K90" si="10">AVERAGE(A87:J87)</f>
+        <v>2.2000000000000006E-3</v>
+      </c>
+      <c r="M87" s="1">
+        <v>0.26479999999999998</v>
+      </c>
+      <c r="N87" s="1">
+        <v>0.26910000000000001</v>
+      </c>
+      <c r="O87" s="1">
+        <v>0.27139999999999997</v>
+      </c>
+      <c r="P87" s="1">
+        <v>0.27339999999999998</v>
+      </c>
+      <c r="Q87" s="1">
+        <v>0.2737</v>
+      </c>
+      <c r="R87" s="1">
+        <v>0.27589999999999998</v>
+      </c>
+      <c r="S87" s="1">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="T87" s="1">
+        <v>0.2782</v>
+      </c>
+      <c r="U87" s="1">
+        <v>0.27850000000000003</v>
+      </c>
+      <c r="V87" s="1">
+        <v>0.28179999999999999</v>
+      </c>
+      <c r="W87" s="3">
+        <f>AVERAGE(M87:V87)*4000</f>
+        <v>1097.92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A88" s="1">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="C88" s="1">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="J88" s="1">
+        <v>0.621</v>
+      </c>
+      <c r="K88" s="5">
+        <f t="shared" si="10"/>
+        <v>0.6472</v>
+      </c>
+      <c r="M88" s="1">
+        <v>0.26479999999999998</v>
+      </c>
+      <c r="N88" s="1">
+        <v>0.26910000000000001</v>
+      </c>
+      <c r="O88" s="1">
+        <v>0.27160000000000001</v>
+      </c>
+      <c r="P88" s="1">
+        <v>0.27339999999999998</v>
+      </c>
+      <c r="Q88" s="1">
+        <v>0.2737</v>
+      </c>
+      <c r="R88" s="1">
+        <v>0.27589999999999998</v>
+      </c>
+      <c r="S88" s="1">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="T88" s="1">
+        <v>0.2782</v>
+      </c>
+      <c r="U88" s="1">
+        <v>0.2787</v>
+      </c>
+      <c r="V88" s="1">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="W88" s="3">
+        <f t="shared" ref="W88:W90" si="11">AVERAGE(M88:V88)*4000</f>
+        <v>1098.1600000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A89" s="1">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.437</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="J89" s="1">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="K89" s="5">
+        <f t="shared" si="10"/>
+        <v>0.4466</v>
+      </c>
+      <c r="M89" s="1">
+        <v>0.30349999999999999</v>
+      </c>
+      <c r="N89" s="1">
+        <v>0.30609999999999998</v>
+      </c>
+      <c r="O89" s="1">
+        <v>0.30780000000000002</v>
+      </c>
+      <c r="P89" s="1">
+        <v>0.31009999999999999</v>
+      </c>
+      <c r="Q89" s="1">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="R89" s="1">
+        <v>0.31419999999999998</v>
+      </c>
+      <c r="S89" s="1">
+        <v>0.31469999999999998</v>
+      </c>
+      <c r="T89" s="1">
+        <v>0.29570000000000002</v>
+      </c>
+      <c r="U89" s="1">
+        <v>0.31490000000000001</v>
+      </c>
+      <c r="V89" s="1">
+        <v>0.32050000000000001</v>
+      </c>
+      <c r="W89" s="3">
+        <f t="shared" si="11"/>
+        <v>1237.0400000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A90" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B90" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C90" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="D90" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E90" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="F90" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G90" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="H90" s="1">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I90" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="J90" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="K90" s="5">
+        <f t="shared" si="10"/>
+        <v>8.4000000000000012E-3</v>
+      </c>
+      <c r="M90" s="1">
+        <v>0.26939999999999997</v>
+      </c>
+      <c r="N90" s="1">
+        <v>0.27160000000000001</v>
+      </c>
+      <c r="O90" s="1">
+        <v>0.27339999999999998</v>
+      </c>
+      <c r="P90" s="1">
+        <v>0.2737</v>
+      </c>
+      <c r="Q90" s="1">
+        <v>0.2757</v>
+      </c>
+      <c r="R90" s="1">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="S90" s="1">
+        <v>0.2782</v>
+      </c>
+      <c r="T90" s="1">
+        <v>0.317</v>
+      </c>
+      <c r="U90" s="1">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="V90" s="1">
+        <v>0.2823</v>
+      </c>
+      <c r="W90" s="3">
+        <f t="shared" si="11"/>
+        <v>1120.5200000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>